<commit_message>
preprocess and MatchReport modify
</commit_message>
<xml_diff>
--- a/data/MatchReport.xlsx
+++ b/data/MatchReport.xlsx
@@ -81,7 +81,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,6 +92,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -128,10 +134,10 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">

</xml_diff>

<commit_message>
Data matchreport update with Goals and cards
</commit_message>
<xml_diff>
--- a/data/MatchReport.xlsx
+++ b/data/MatchReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\ARGENTINA_INF8808_PROJET\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Videos\DataViz\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8DEB21F1-6E22-4D7C-AF88-1B7C38D14D05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADDFDC1A-18BA-4D7B-9016-1958D373A27F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="288" windowWidth="13704" windowHeight="10368" xr2:uid="{F60D035B-A79A-470D-AD71-2BD4DA331F5F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{F60D035B-A79A-470D-AD71-2BD4DA331F5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Match Report" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Opponent</t>
   </si>
@@ -84,6 +84,18 @@
   </si>
   <si>
     <t>Croatia</t>
+  </si>
+  <si>
+    <t>Cards For Argentina</t>
+  </si>
+  <si>
+    <t>Cards For Opponent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goal For Argentina </t>
+  </si>
+  <si>
+    <t>Goal Against Argentina</t>
   </si>
 </sst>
 </file>
@@ -435,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01228636-8058-47EE-9ADE-BCC84870E835}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" activeCellId="1" sqref="C16 B13"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -451,9 +463,12 @@
     <col min="7" max="7" width="28.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -481,8 +496,20 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -510,8 +537,20 @@
       <c r="I2">
         <v>100</v>
       </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>6</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -539,8 +578,20 @@
       <c r="I3">
         <v>0</v>
       </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>4</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -568,8 +619,20 @@
       <c r="I4">
         <v>80</v>
       </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -597,8 +660,20 @@
       <c r="I5">
         <v>60</v>
       </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -626,8 +701,20 @@
       <c r="I6">
         <v>75</v>
       </c>
+      <c r="J6">
+        <v>10</v>
+      </c>
+      <c r="K6">
+        <v>10</v>
+      </c>
+      <c r="L6">
+        <v>6</v>
+      </c>
+      <c r="M6">
+        <v>5</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -655,8 +742,20 @@
       <c r="I7">
         <v>66</v>
       </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>2</v>
+      </c>
+      <c r="L7">
+        <v>3</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -683,6 +782,18 @@
       </c>
       <c r="I8">
         <v>77</v>
+      </c>
+      <c r="J8">
+        <v>5</v>
+      </c>
+      <c r="K8">
+        <v>3</v>
+      </c>
+      <c r="L8">
+        <v>7</v>
+      </c>
+      <c r="M8">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Heatmap and lolipop modify --- Lolipop not yet good
</commit_message>
<xml_diff>
--- a/data/MatchReport.xlsx
+++ b/data/MatchReport.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Videos\DataViz\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85AFEB0-CCDB-420F-A885-9614DD274ED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Match Report" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Match Report"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -55,6 +49,12 @@
     <t>Goal Against Argentina</t>
   </si>
   <si>
+    <t>Goal per Shot For Argentina</t>
+  </si>
+  <si>
+    <t>Goal per Shot Against Argentina</t>
+  </si>
+  <si>
     <t>Saudi Arabia</t>
   </si>
   <si>
@@ -74,18 +74,13 @@
   </si>
   <si>
     <t>France</t>
-  </si>
-  <si>
-    <t>Goal per Shot For Argentina</t>
-  </si>
-  <si>
-    <t>Goal per Shot Against Argentina</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -96,13 +91,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -134,36 +129,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="8">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -174,10 +171,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -215,71 +212,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -307,7 +304,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -330,11 +327,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -343,13 +340,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -359,7 +356,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -368,7 +365,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -377,7 +374,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -385,10 +382,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -453,76 +450,75 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="23.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="21.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="24.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="26.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="29.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="25.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="6" width="28.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="6" width="17.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="6" width="20.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="6" width="19.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="7" width="23.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="7" width="23.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>19</v>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>11</v>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="B2" s="2">
         <v>69</v>
@@ -554,16 +550,16 @@
       <c r="K2" s="2">
         <v>2</v>
       </c>
-      <c r="L2" s="5">
-        <v>0</v>
-      </c>
-      <c r="M2" s="5">
+      <c r="L2" s="2">
+        <v>0</v>
+      </c>
+      <c r="M2" s="3">
         <v>0.67</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>12</v>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B3" s="2">
         <v>58</v>
@@ -595,16 +591,16 @@
       <c r="K3" s="2">
         <v>0</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="4">
         <v>0.4</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>13</v>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="B4" s="2">
         <v>73</v>
@@ -636,16 +632,16 @@
       <c r="K4" s="2">
         <v>0</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="3">
         <v>0.09</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>14</v>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B5" s="2">
         <v>60</v>
@@ -677,16 +673,16 @@
       <c r="K5" s="2">
         <v>1</v>
       </c>
-      <c r="L5" s="5">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="M5" s="5">
+      <c r="L5" s="3">
+        <v>0.14</v>
+      </c>
+      <c r="M5" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>15</v>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="B6" s="2">
         <v>48</v>
@@ -718,16 +714,16 @@
       <c r="K6" s="2">
         <v>5</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="3">
         <v>0.08</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="3">
         <v>0.33</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>16</v>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B7" s="2">
         <v>40</v>
@@ -759,16 +755,16 @@
       <c r="K7" s="2">
         <v>0</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="3">
         <v>0.25</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>17</v>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+      <c r="A8" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="B8" s="2">
         <v>54</v>
@@ -800,10 +796,10 @@
       <c r="K8" s="2">
         <v>5</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="3">
         <v>0.11</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="3">
         <v>0.13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Data for Goal change to exclude penalty goals of each ,match
</commit_message>
<xml_diff>
--- a/data/MatchReport.xlsx
+++ b/data/MatchReport.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Videos\DataViz\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774B15D8-C767-4378-8560-807B6F84CA50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Match Report"/>
+    <sheet name="Match Report" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -79,8 +85,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -129,38 +134,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -171,10 +173,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -212,71 +214,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -304,7 +306,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -327,11 +329,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -340,13 +342,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -356,7 +358,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -365,7 +367,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -374,7 +376,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -382,10 +384,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -450,356 +452,357 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="21.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="24.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="26.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="29.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="6" width="25.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="6" width="28.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="6" width="17.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="6" width="20.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="6" width="19.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="7" width="23.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="7" width="23.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="23.5546875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>69</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>31</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>83</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>66</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="1">
         <v>36</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="1">
         <v>67</v>
       </c>
-      <c r="H2" s="2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="2">
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
         <v>100</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="1">
         <v>1</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="1">
         <v>2</v>
       </c>
-      <c r="L2" s="2">
-        <v>0</v>
-      </c>
-      <c r="M2" s="3">
+      <c r="L2" s="1">
+        <v>0</v>
+      </c>
+      <c r="M2" s="2">
         <v>0.67</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>58</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>42</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>83</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>74</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>40</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <v>25</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="1">
         <v>100</v>
       </c>
-      <c r="I3" s="2">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2">
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
         <v>2</v>
       </c>
-      <c r="K3" s="2">
-        <v>0</v>
-      </c>
-      <c r="L3" s="4">
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
         <v>0.4</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3" s="1">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>73</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>27</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>91</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>77</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>45</v>
       </c>
-      <c r="G4" s="2">
-        <v>0</v>
-      </c>
-      <c r="H4" s="2">
-        <v>0</v>
-      </c>
-      <c r="I4" s="2">
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
         <v>80</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="1">
         <v>2</v>
       </c>
-      <c r="K4" s="2">
-        <v>0</v>
-      </c>
-      <c r="L4" s="3">
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
         <v>0.09</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="1">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>60</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>40</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>87</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>81</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>36</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <v>20</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="1">
         <v>100</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="1">
         <v>60</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="1">
         <v>2</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="1">
         <v>1</v>
       </c>
-      <c r="L5" s="3">
-        <v>0.14</v>
-      </c>
-      <c r="M5" s="2">
+      <c r="L5" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M5" s="1">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>48</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>52</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>82</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>82</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>31</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <v>33</v>
       </c>
-      <c r="H6" s="2">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2">
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
         <v>75</v>
       </c>
-      <c r="J6" s="2">
-        <v>6</v>
-      </c>
-      <c r="K6" s="2">
-        <v>5</v>
-      </c>
-      <c r="L6" s="3">
+      <c r="J6" s="1">
+        <v>2</v>
+      </c>
+      <c r="K6" s="1">
+        <v>2</v>
+      </c>
+      <c r="L6" s="2">
         <v>0.08</v>
       </c>
-      <c r="M6" s="3">
+      <c r="M6" s="2">
         <v>0.33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>40</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>60</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>82</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>85</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <v>75</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
         <v>17</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="1">
         <v>100</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="1">
         <v>66</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="1">
         <v>3</v>
       </c>
-      <c r="K7" s="2">
-        <v>0</v>
-      </c>
-      <c r="L7" s="3">
+      <c r="K7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="2">
         <v>0.25</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7" s="1">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>54</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>46</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>80</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>74</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
         <v>47</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="1">
         <v>38</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="1">
         <v>66</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="1">
         <v>77</v>
       </c>
-      <c r="J8" s="2">
-        <v>7</v>
-      </c>
-      <c r="K8" s="2">
-        <v>5</v>
-      </c>
-      <c r="L8" s="3">
+      <c r="J8" s="1">
+        <v>3</v>
+      </c>
+      <c r="K8" s="1">
+        <v>3</v>
+      </c>
+      <c r="L8" s="2">
         <v>0.11</v>
       </c>
-      <c r="M8" s="3">
+      <c r="M8" s="2">
         <v>0.13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
error with Goal for attempt to resolve
</commit_message>
<xml_diff>
--- a/data/MatchReport.xlsx
+++ b/data/MatchReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Videos\DataViz\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774B15D8-C767-4378-8560-807B6F84CA50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295DA566-B750-4E8A-83DC-4E6DD7DB362F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,9 +49,6 @@
     <t>Saves Against Argentina</t>
   </si>
   <si>
-    <t xml:space="preserve">Goal For Argentina </t>
-  </si>
-  <si>
     <t>Goal Against Argentina</t>
   </si>
   <si>
@@ -80,6 +77,9 @@
   </si>
   <si>
     <t>France</t>
+  </si>
+  <si>
+    <t>Goal For Argentina</t>
   </si>
 </sst>
 </file>
@@ -134,7 +134,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -150,6 +150,9 @@
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -459,7 +462,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -472,8 +475,8 @@
     <col min="6" max="6" width="25.44140625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.21875" style="4" customWidth="1"/>
     <col min="11" max="11" width="19.44140625" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="23.5546875" style="5" bestFit="1" customWidth="1"/>
   </cols>
@@ -506,22 +509,22 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1">
         <v>69</v>
@@ -562,7 +565,7 @@
     </row>
     <row r="3" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1">
         <v>58</v>
@@ -603,7 +606,7 @@
     </row>
     <row r="4" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1">
         <v>73</v>
@@ -644,7 +647,7 @@
     </row>
     <row r="5" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1">
         <v>60</v>
@@ -685,7 +688,7 @@
     </row>
     <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1">
         <v>48</v>
@@ -726,7 +729,7 @@
     </row>
     <row r="7" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1">
         <v>40</v>
@@ -767,7 +770,7 @@
     </row>
     <row r="8" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1">
         <v>54</v>

</xml_diff>